<commit_message>
delete some trashy files
</commit_message>
<xml_diff>
--- a/CDN.xlsx
+++ b/CDN.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mengjiaying/INFOCOM_2021/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3D746AE9-09C6-B14E-8B5D-71AB94F2615A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45B01BDF-E840-8544-BF63-413B3DDFF16B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="460" windowWidth="28240" windowHeight="16460" xr2:uid="{8E72F94A-A293-584E-A65C-31121CF5049F}"/>
+    <workbookView xWindow="1960" yWindow="4720" windowWidth="28240" windowHeight="16460" xr2:uid="{8E72F94A-A293-584E-A65C-31121CF5049F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1885,7 +1885,7 @@
   <dimension ref="A1:D449"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E310" sqref="E310"/>
+      <selection activeCell="H72" sqref="H72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2501,7 +2501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" ht="12">
       <c r="A55" t="s">
         <v>27</v>
       </c>
@@ -2515,7 +2515,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" ht="1" customHeight="1">
       <c r="A56" t="s">
         <v>27</v>
       </c>

</xml_diff>